<commit_message>
Catching up to main changes
</commit_message>
<xml_diff>
--- a/docs/DOD_SprintA_V1.xlsx
+++ b/docs/DOD_SprintA_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredmatthews/McGill/McGill Winter 2023/ECSE 428/StuddyBuddy/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Projects\StuddyBuddy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBE1BC2B-8D27-E847-A654-A736BB1C455A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0060C2-CEE9-4E9E-9DD9-182E0F08770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31300" yWindow="2120" windowWidth="28040" windowHeight="17440" xr2:uid="{5BC7BDE3-1049-5D46-B5F2-3FAEB4CF86CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5BC7BDE3-1049-5D46-B5F2-3FAEB4CF86CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,13 +87,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,7 +121,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -133,6 +139,934 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36945E63-81F3-AB47-653D-6681EA431D20}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E83365-1FF6-2E1E-BD11-4A6F9C8EC3EB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F41986-AF49-6999-E223-CDC0580682A4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{640EBFF3-E3A7-A821-D591-B6AA10A129B3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C338E916-39F7-C8E6-5FD8-6150CCC61904}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68EC761-51B9-C404-7453-8A76F25E2A4F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE5D0276-5A72-2A9F-BB72-7D9F87A598B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1034"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D69BCB5-5A05-B6F0-19A4-EBDADDFBE423}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{828829A0-C408-5260-E837-06F0028CE805}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1036"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36FAA2F9-4D41-30A8-4EB1-4A835357BE7F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1037"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31E85B47-9D73-71A2-6E19-D0404284770F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>352425</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1038"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11489583-100C-D02E-69F8-D47B6F2CEEFE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,89 +1365,457 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B619F26-384C-E04B-A730-F08B9AFB243F}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B619F26-384C-E04B-A730-F08B9AFB243F}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId3" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId4" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId5" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId6" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId7" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId8" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId9" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId10" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId11" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId12" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId13" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1037" r:id="rId14" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1038" r:id="rId15" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>352425</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>